<commit_message>
jdre-17/03/2015-Se actualizo el DICCIONARIO_DE_DATOS.xlsx de acorde a las modificaciones establecidas en la base de datos.
</commit_message>
<xml_diff>
--- a/ afgmx/AFGMX/PROCESO_DESARROLLO/F3_ANALISIS_Y_DISENO/MO_DATOS/DICCIONARIO_DE_DATOS.xlsx
+++ b/ afgmx/AFGMX/PROCESO_DESARROLLO/F3_ANALISIS_Y_DISENO/MO_DATOS/DICCIONARIO_DE_DATOS.xlsx
@@ -5,32 +5,33 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diegox\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diegox\Desktop\Proyecto\AFGMX\PROCESO_DESARROLLO\F3_ANALISIS_Y_DISENO\MO_DATOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="4" r:id="rId1"/>
     <sheet name="Hoja15" sheetId="21" state="hidden" r:id="rId2"/>
     <sheet name="Hoja16" sheetId="22" state="hidden" r:id="rId3"/>
     <sheet name="Hoja17" sheetId="23" state="hidden" r:id="rId4"/>
-    <sheet name="History" sheetId="30" r:id="rId5"/>
-    <sheet name="soil_type" sheetId="5" r:id="rId6"/>
-    <sheet name="Weather_data" sheetId="3" r:id="rId7"/>
-    <sheet name="Hoja1" sheetId="9" state="hidden" r:id="rId8"/>
-    <sheet name="Hoja2" sheetId="10" state="hidden" r:id="rId9"/>
-    <sheet name="Hoja3" sheetId="11" state="hidden" r:id="rId10"/>
-    <sheet name="Hoja4" sheetId="12" state="hidden" r:id="rId11"/>
-    <sheet name="Hoja5" sheetId="13" state="hidden" r:id="rId12"/>
-    <sheet name="Hoja6" sheetId="14" state="hidden" r:id="rId13"/>
-    <sheet name="Hoja9" sheetId="15" state="hidden" r:id="rId14"/>
-    <sheet name="Hoja12" sheetId="18" state="hidden" r:id="rId15"/>
-    <sheet name="Hoja13" sheetId="19" state="hidden" r:id="rId16"/>
-    <sheet name="Hoja14" sheetId="20" state="hidden" r:id="rId17"/>
-    <sheet name="Hoja10" sheetId="16" state="hidden" r:id="rId18"/>
-    <sheet name="Hoja11" sheetId="17" state="hidden" r:id="rId19"/>
+    <sheet name="weather" sheetId="3" r:id="rId5"/>
+    <sheet name="alture" sheetId="31" r:id="rId6"/>
+    <sheet name="Citys" sheetId="32" r:id="rId7"/>
+    <sheet name="humidity" sheetId="33" r:id="rId8"/>
+    <sheet name="Hoja1" sheetId="9" state="hidden" r:id="rId9"/>
+    <sheet name="Hoja2" sheetId="10" state="hidden" r:id="rId10"/>
+    <sheet name="Hoja3" sheetId="11" state="hidden" r:id="rId11"/>
+    <sheet name="Hoja4" sheetId="12" state="hidden" r:id="rId12"/>
+    <sheet name="Hoja5" sheetId="13" state="hidden" r:id="rId13"/>
+    <sheet name="Hoja6" sheetId="14" state="hidden" r:id="rId14"/>
+    <sheet name="Hoja9" sheetId="15" state="hidden" r:id="rId15"/>
+    <sheet name="Hoja12" sheetId="18" state="hidden" r:id="rId16"/>
+    <sheet name="Hoja13" sheetId="19" state="hidden" r:id="rId17"/>
+    <sheet name="Hoja14" sheetId="20" state="hidden" r:id="rId18"/>
+    <sheet name="Hoja10" sheetId="16" state="hidden" r:id="rId19"/>
+    <sheet name="Hoja11" sheetId="17" state="hidden" r:id="rId20"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="67">
   <si>
     <t>Campo</t>
   </si>
@@ -107,9 +108,6 @@
     <t>BigInt</t>
   </si>
   <si>
-    <t>firstname</t>
-  </si>
-  <si>
     <t>Nombre(s) del usuario</t>
   </si>
   <si>
@@ -155,78 +153,9 @@
     <t>Dira si la cuenta esta activa o esta dada de baja</t>
   </si>
   <si>
-    <t>History</t>
-  </si>
-  <si>
-    <t>Permite almacenar la información de las acciones que realice el usuario.</t>
-  </si>
-  <si>
-    <t>idHistory</t>
-  </si>
-  <si>
-    <t>Clave unica que identifica al historial.</t>
-  </si>
-  <si>
-    <t>date_Act</t>
-  </si>
-  <si>
-    <t>Fecha en que se realizo</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>hour_Act</t>
-  </si>
-  <si>
-    <t>Hora en que se realizo</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>activity</t>
-  </si>
-  <si>
-    <t>Descripcion de la actividad</t>
-  </si>
-  <si>
-    <t>clave del usuario propietario de este historial</t>
-  </si>
-  <si>
-    <t>idType</t>
-  </si>
-  <si>
-    <t>Soil_type</t>
-  </si>
-  <si>
-    <t>Permite almacenar la información de los tipos de suelos.</t>
-  </si>
-  <si>
-    <t>Clave unica que identifica al tipo de suelo.</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>nombre del tipo de suelo.</t>
-  </si>
-  <si>
-    <t>features</t>
-  </si>
-  <si>
-    <t>Descripcion del tipo.</t>
-  </si>
-  <si>
-    <t>PH</t>
-  </si>
-  <si>
-    <t>Es una medida de acidez o alcalinidad de una disolución.</t>
-  </si>
-  <si>
-    <t>Weather_data</t>
-  </si>
-  <si>
     <t>Permite almacenar la información del clima.</t>
   </si>
   <si>
@@ -236,29 +165,92 @@
     <t>Clave unica que identifica al clima.</t>
   </si>
   <si>
-    <t>Maximun_temp</t>
-  </si>
-  <si>
-    <t>Temperatura maxima.</t>
-  </si>
-  <si>
-    <t>Minimun_temp</t>
-  </si>
-  <si>
-    <t>Temperatura minima.</t>
-  </si>
-  <si>
-    <t>Wind_speed</t>
-  </si>
-  <si>
-    <t>Velocidad del viento</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>clouds</t>
+  </si>
+  <si>
+    <t>idCity</t>
+  </si>
+  <si>
+    <t>dateRegistry</t>
+  </si>
+  <si>
+    <t>Temperatura.</t>
+  </si>
+  <si>
+    <t>Nubocidad.</t>
+  </si>
+  <si>
+    <t>Clave que enlaza a la ciudad correspondiente.</t>
+  </si>
+  <si>
+    <t>Fecha en que se registro esos datos.</t>
+  </si>
+  <si>
+    <t>weather</t>
+  </si>
+  <si>
+    <t>alture</t>
+  </si>
+  <si>
+    <t>Permite almacenar informacion sobre la altura donde se encuentra el punto a solicitar la informacion.</t>
+  </si>
+  <si>
+    <t>idAlture</t>
+  </si>
+  <si>
+    <t>Clave unica que identifica la altura.</t>
+  </si>
+  <si>
+    <t>Valor de la altura.</t>
+  </si>
+  <si>
+    <t>Decimal(10,2)</t>
+  </si>
+  <si>
+    <t>Citys</t>
+  </si>
+  <si>
+    <t>Clave unica que identifica la ciudad.</t>
+  </si>
+  <si>
+    <t>Permite almacenar informacion sobre la ciudad y ciudades.</t>
+  </si>
+  <si>
+    <t>Nombre de la ciudad.</t>
+  </si>
+  <si>
+    <t>humidity</t>
+  </si>
+  <si>
+    <t>idHumidity</t>
+  </si>
+  <si>
+    <t>Permite almacenar informacion sobre la humedad.</t>
+  </si>
+  <si>
+    <t>Clave unica que identifica el registro de la humedad.</t>
+  </si>
+  <si>
+    <t>percentaje</t>
+  </si>
+  <si>
+    <t>Porcentaje de humedad-</t>
+  </si>
+  <si>
+    <t>varchar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,12 +273,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -321,11 +307,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -374,7 +359,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla41513" displayName="Tabla41513" ref="A3:K8" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla48" displayName="Tabla48" ref="A3:K8" totalsRowShown="0">
   <autoFilter ref="A3:K8"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Campo"/>
@@ -394,7 +379,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla412" displayName="Tabla412" ref="A3:K7" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla482" displayName="Tabla482" ref="A3:K7" totalsRowShown="0">
   <autoFilter ref="A3:K7"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Campo"/>
@@ -414,8 +399,28 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla48" displayName="Tabla48" ref="A3:K8" totalsRowShown="0">
-  <autoFilter ref="A3:K8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla4823" displayName="Tabla4823" ref="A3:K5" totalsRowShown="0">
+  <autoFilter ref="A3:K5"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Campo"/>
+    <tableColumn id="2" name="Descripción"/>
+    <tableColumn id="3" name="Tipo"/>
+    <tableColumn id="4" name="Longitud"/>
+    <tableColumn id="5" name="Llave primaria"/>
+    <tableColumn id="6" name="Llave foránea"/>
+    <tableColumn id="7" name="Autoincremento"/>
+    <tableColumn id="8" name="Default"/>
+    <tableColumn id="9" name="Acepta valores nulos"/>
+    <tableColumn id="10" name="Único"/>
+    <tableColumn id="11" name="Índice"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla4824" displayName="Tabla4824" ref="A3:K7" totalsRowShown="0">
+  <autoFilter ref="A3:K7"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Campo"/>
     <tableColumn id="2" name="Descripción"/>
@@ -698,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,34 +714,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -804,10 +809,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -836,10 +841,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -868,10 +873,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -900,10 +905,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -932,10 +937,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -964,10 +969,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -996,10 +1001,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -1028,10 +1033,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
         <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -1206,6 +1211,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -1234,110 +1251,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="A1:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="53" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>20</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1346,10 +1363,10 @@
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -1372,13 +1389,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -1401,22 +1418,19 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
         <v>47</v>
       </c>
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
       <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>500</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
@@ -1433,22 +1447,19 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
         <v>12</v>
@@ -1480,448 +1491,203 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="K7" sqref="A1:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>100</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>500</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1937,15 +1703,377 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="54.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>